<commit_message>
add some yale results
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/experiments_yale.xlsx
+++ b/examples/masterarbeit/experiments_yale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23689FAD-A0A2-49C7-ABD8-5DCEB1C497BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA88DDF-B454-4174-B3BD-42EE539A3CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="41">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -120,23 +120,47 @@
     <t>1,4,5,6,9,10,19,20</t>
   </si>
   <si>
-    <t>exp_yale_20200114-104429</t>
-  </si>
-  <si>
-    <t>ONGOING</t>
-  </si>
-  <si>
     <t>exp_yale_20200116-123756</t>
   </si>
   <si>
     <t>exp_yale_20200116-180854</t>
+  </si>
+  <si>
+    <t>exp_yale_20200116-104619</t>
+  </si>
+  <si>
+    <t>exp_yale_20200117-171139</t>
+  </si>
+  <si>
+    <t>exp_yale_20200117-095427</t>
+  </si>
+  <si>
+    <t>exp_yale_20200119-094913</t>
+  </si>
+  <si>
+    <t>NO RESULT - TO FEW BATCHES</t>
+  </si>
+  <si>
+    <t>unnötig?</t>
+  </si>
+  <si>
+    <t>funktioniert, overfitted aber irgendwann</t>
+  </si>
+  <si>
+    <t>funktioniert</t>
+  </si>
+  <si>
+    <t>funktioniert, number total batches: 6, number of malicious batches: 3</t>
+  </si>
+  <si>
+    <t>ONGOING (exp_yale_20200120-125642)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +196,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +226,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -215,21 +263,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="4" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -558,7 +619,7 @@
     <col min="7" max="7" width="18.15234375" customWidth="1"/>
     <col min="8" max="8" width="12.69140625" customWidth="1"/>
     <col min="9" max="9" width="3.3046875" customWidth="1"/>
-    <col min="10" max="10" width="30.3046875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="37.3046875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -789,7 +850,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -818,7 +879,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -1084,7 +1145,7 @@
         <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -1177,7 +1238,7 @@
       </c>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +1264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1229,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1256,7 +1317,7 @@
       </c>
       <c r="J35"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1267,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1283,7 +1344,7 @@
       </c>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1371,7 @@
       </c>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1338,19 +1399,24 @@
       <c r="J38" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K38" s="6"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1376,7 +1442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1468,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -1428,7 +1494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1455,19 +1521,19 @@
       </c>
       <c r="J45"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="J46"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>21</v>
       </c>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1494,7 +1560,7 @@
       </c>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1521,7 +1587,7 @@
       </c>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -1548,212 +1614,259 @@
       </c>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B52" s="3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="1">
         <v>4</v>
       </c>
-      <c r="C52" s="3">
-        <v>1</v>
-      </c>
-      <c r="D52" s="3">
-        <v>8</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>32</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="1">
+        <v>50</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="3">
+      <c r="H54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="1">
         <v>4</v>
       </c>
-      <c r="C53" s="3">
-        <v>1</v>
-      </c>
-      <c r="D53" s="3">
-        <v>8</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="3">
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>32</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="1">
+        <v>100</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="H55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58">
         <v>25</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B54" s="3">
-        <v>4</v>
-      </c>
-      <c r="C54" s="3">
-        <v>1</v>
-      </c>
-      <c r="D54" s="3">
-        <v>8</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="3">
+      <c r="G58" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="5">
+        <v>9</v>
+      </c>
+      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5">
+        <v>8</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="5">
         <v>50</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G59" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J54"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="3">
-        <v>4</v>
-      </c>
-      <c r="C55" s="3">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3">
-        <v>8</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="3">
-        <v>75</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="H59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <v>100</v>
+      </c>
+      <c r="G60" t="s">
         <v>25</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J55"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="3">
-        <v>4</v>
-      </c>
-      <c r="C56" s="3">
-        <v>1</v>
-      </c>
-      <c r="D56" s="3">
-        <v>8</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="3">
+      <c r="H60" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="9">
+        <v>9</v>
+      </c>
+      <c r="C62" s="9">
+        <v>1</v>
+      </c>
+      <c r="D62" s="9">
+        <v>32</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="9">
+        <v>25</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="9">
+        <v>9</v>
+      </c>
+      <c r="C63" s="9">
+        <v>1</v>
+      </c>
+      <c r="D63" s="9">
+        <v>32</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="9">
+        <v>50</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="1">
+        <v>9</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>32</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1">
         <v>100</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G64" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J56"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B57" s="3">
-        <v>6</v>
-      </c>
-      <c r="C57" s="3">
-        <v>1</v>
-      </c>
-      <c r="D57" s="3">
-        <v>8</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57" s="3">
-        <v>50</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J57"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="3">
-        <v>6</v>
-      </c>
-      <c r="C58" s="3">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3">
-        <v>8</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="3">
-        <v>100</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J59"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J60"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J61"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J64"/>
+      <c r="H64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="65" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J65"/>
@@ -1772,6 +1885,24 @@
     </row>
     <row r="70" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J70"/>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J71"/>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J72"/>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J73"/>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J74"/>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J75"/>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>